<commit_message>
output directory for new changes
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ndh-CareTeam.xlsx
+++ b/output/StructureDefinition-ndh-CareTeam.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-20T20:37:10-04:00</t>
+    <t>2022-10-31T22:12:57-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -438,7 +438,7 @@
     <t>alias</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/careteam-alias}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-careteam-alias}
 </t>
   </si>
   <si>
@@ -455,7 +455,7 @@
     <t>location</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/location-reference}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-location-reference}
 </t>
   </si>
   <si>
@@ -468,7 +468,7 @@
     <t>service</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/healthcareservice-reference}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-healthcareservice-reference}
 </t>
   </si>
   <si>
@@ -481,7 +481,7 @@
     <t>endpoint</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/endpoint-reference}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-endpoint-reference}
 </t>
   </si>
   <si>
@@ -494,7 +494,7 @@
     <t>restriction</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/usage-restriction}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-usage-restriction}
 </t>
   </si>
   <si>
@@ -581,7 +581,7 @@
     <t>status</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/identifier-status}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-identifier-status}
 </t>
   </si>
   <si>
@@ -1064,7 +1064,7 @@
     <t>contactpoint-availabletime</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/contactpoint-availabletime}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-contactpoint-availabletime}
 </t>
   </si>
   <si>
@@ -1077,7 +1077,7 @@
     <t>via-intermediary</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/via-intermediary}
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/us/ndh/StructureDefinition/base-ext-via-intermediary}
 </t>
   </si>
   <si>

</xml_diff>